<commit_message>
Data Extraction in Spreadsheet using UiPath
</commit_message>
<xml_diff>
--- a/Process/ExtractedData.xlsx
+++ b/Process/ExtractedData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Process\Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F4C1E2-5616-42C3-BC12-C7975F44A4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C708902-73B5-47AF-83DB-B54712F9A682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="5136" windowWidth="13440" windowHeight="6804" xr2:uid="{9226592C-126F-4DDD-B51D-DE679A53EDC7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9226592C-126F-4DDD-B51D-DE679A53EDC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,297 +25,282 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
-  <si>
-    <t>Clothing and</t>
-  </si>
-  <si>
-    <t>Filters Home Bottomwear Jeans</t>
-  </si>
-  <si>
-    <t>Showing 1 – 40 of Accessories 14,627 results for "JEANS "</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="92">
   <si>
     <t>CATEGORIES Sort By Relevance Popularity Price -- Low to High Price -- High to Low Newest First</t>
   </si>
   <si>
-    <t>Accessories Bottomwear</t>
-  </si>
-  <si>
-    <t>Jeans</t>
-  </si>
-  <si>
-    <t>Women's Jeans</t>
-  </si>
-  <si>
-    <t>Kids' Jeans</t>
-  </si>
-  <si>
-    <t>Men's Jeans</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>. . . . . . .</t>
-  </si>
-  <si>
-    <t>MinMin to ₹1500+₹1500+</t>
-  </si>
-  <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>Fit</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>Distress BEN Men MARTIN Regular Mid Rise Black LEVI512 'S Men Regular Mid Rise KOTTY Women Regular High Rise KOTTY Women Flared High Rise</t>
-  </si>
-  <si>
-    <t>Jeans Blue Jeans Grey Jeans Black Jeans</t>
-  </si>
-  <si>
-    <t>Fade 83% 50% 83% 75% ₹499 ₹2,999 off ₹1,449 ₹2,899 off ₹499 ₹2,999 off ₹499 ₹1,999 off</t>
-  </si>
-  <si>
-    <t>Free delivery Free delivery Free delivery Free delivery</t>
-  </si>
-  <si>
-    <t>Theme Hot Summer Deal Hot Summer Deal Hot Deal Hot Deal</t>
-  </si>
-  <si>
-    <t>Offers</t>
-  </si>
-  <si>
-    <t>Buy More, Save More</t>
-  </si>
-  <si>
-    <t>Special Price</t>
-  </si>
-  <si>
-    <t>Pack of</t>
-  </si>
-  <si>
-    <t>Availability</t>
-  </si>
-  <si>
-    <t>KOTTY Women Regular High Rise KOTTY Women Flared Mid Rise Blue TYFFYN Women Slim High Rise Black NAMMA Men &amp; OORU Women TREND Slim Mid Rise</t>
-  </si>
-  <si>
-    <t>Black Jeans 83% Jeans 75% Jeans 70% Black Jeans 73%</t>
-  </si>
-  <si>
-    <t>₹499 ₹2,999 off ₹499 ₹1,999 off ₹449 ₹1,499 off ₹444 ₹1,699 off</t>
-  </si>
-  <si>
-    <t>Hot Deal Hot Deal</t>
-  </si>
-  <si>
-    <t>Passion Men Slim Mid Rise Blue Urbano Men Fashion Slim Mid Rise Black KILLER Men Slim Mid Rise Black KILLER Men Skinny Mid Rise Dark</t>
-  </si>
-  <si>
-    <t>Jeans 80% Jeans 50% Jeans 55% Blue Jeans 65%</t>
-  </si>
-  <si>
-    <t>₹559 ₹2,799 off ₹591 ₹1,199 off ₹1,574 ₹3,499 off ₹1,224 ₹3,499 off</t>
-  </si>
-  <si>
-    <t>Hot Summer Deal Hot Deal Buy 2 items, save extra 5% Hot Summer Deal</t>
-  </si>
-  <si>
-    <t>BEN Men MARTIN Regular Mid Rise Grey KILLER Men Slim Mid Rise Dark Blue KOTTY Women Regular High Rise KOTTY Women Flared High Rise</t>
-  </si>
-  <si>
-    <t>Jeans 83% Jeans 65% Black Jeans 83% Grey Jeans 75%</t>
-  </si>
-  <si>
-    <t>₹499 ₹2,999 off ₹1,259 ₹3,599 off ₹499 ₹2,999 off ₹499 ₹1,999 off</t>
-  </si>
-  <si>
-    <t>Hot Summer Deal Hot Summer Deal Hot Deal Hot Deal</t>
-  </si>
-  <si>
-    <t>KOTTY Women Regular Mid Rise LEVI'S Women Skinny High Rise KOTTY Women Slim High Rise Black Emerge Men &amp; World Women Jogger Fit</t>
-  </si>
-  <si>
-    <t>Blue Jeans 76% Blue Jeans 52% Jeans 75% Mid Rise Blue Jeans 50%</t>
-  </si>
-  <si>
-    <t>₹935 ₹3,999 off ₹1,391 ₹2,899 off ₹499 ₹1,999 off ₹299 ₹599 off</t>
-  </si>
-  <si>
-    <t>Hot Deal Buy ₹3000 more, save extra 10% Hot Deal</t>
-  </si>
-  <si>
-    <t>BEING Men HUMAN Regular Mid Rise Black LEVI511 'S Men Slim Mid Rise Blue HIGHLANDER Men Tapered Fit Mid Rise BEN Men MARTIN Regular Mid Rise White</t>
-  </si>
-  <si>
-    <t>Jeans 70% Jeans 50% Black Jeans 51% Jeans 83%</t>
-  </si>
-  <si>
-    <t>₹989 ₹3,299 off ₹1,599 ₹3,199 off ₹685 ₹1,399 off ₹499 ₹2,999 off</t>
-  </si>
-  <si>
-    <t>Lowest Price in 15 days Buy 2 items, save extra 5% Buy 2 items, save extra 5% Hot Summer Deal</t>
-  </si>
-  <si>
-    <t>BEN Men MARTIN Regular Mid Rise White Highlander Men Regular Mid Rise Black KOTTY Women Flared High Rise KOTTY Women Slim High Rise Grey</t>
-  </si>
-  <si>
-    <t>Jeans 83% Jeans 44% Blue Jeans 73% Jeans 75%</t>
-  </si>
-  <si>
-    <t>₹499 ₹2,999 off ₹727 ₹1,299 off ₹499 ₹1,899 off ₹499 ₹1,999 off</t>
-  </si>
-  <si>
-    <t>Hot Summer Deal Buy 2 items, save extra 5% Hot Deal Hot Deal</t>
-  </si>
-  <si>
-    <t>KOTTY Women Regular High Rise TYFFYN Women Slim High Rise Blue KOTTY Women Flared High Rise HRYFiNE Men &amp; Women Slim Mid Rise</t>
-  </si>
-  <si>
-    <t>Grey Jeans 75% Jeans 70% Blue Jeans 75% Black Jeans 67%</t>
-  </si>
-  <si>
-    <t>₹499 ₹1,999 off ₹449 ₹1,499 off ₹499 ₹1,999 off ₹419 ₹1,299 off</t>
-  </si>
-  <si>
-    <t>Hot Deal Lowest Price in 15 days Hot Deal</t>
-  </si>
-  <si>
-    <t>LEVI512 'S Men Tapered Fit Mid Roadster Men Skinny Mid Rise Blue KILLER Men Slim Mid Rise Blue LEVI511 'S Men Slim Mid Rise Grey</t>
-  </si>
-  <si>
-    <t>Rise Black Jeans 45% Jeans 55% Jeans 60% Jeans 50%</t>
-  </si>
-  <si>
-    <t>₹1,759 ₹3,199 off ₹846 ₹1,899 off ₹1,319 ₹3,299 off ₹1,599 ₹3,199 off</t>
-  </si>
-  <si>
-    <t>Buy 2 items, save extra 5% Buy 2 items, save extra 5% Hot Summer Deal</t>
-  </si>
-  <si>
-    <t>Page 1 of 366 1 2 3 4 5 6 7 8 9 10 Next</t>
-  </si>
-  <si>
     <t>Did you find what you were looking for? Yes No</t>
   </si>
   <si>
-    <t>Reviews for Popular Jeans</t>
-  </si>
-  <si>
-    <t>1. LEVI'S 512 Regular Men Blue... Most Helpful Review Recent Review</t>
-  </si>
-  <si>
-    <t>4.2 617 Ratings 50% &amp; 50 Reviews 5 Simply awesome 5 Awesome</t>
-  </si>
-  <si>
-    <t>₹1,449 off Value for money. Perfect product. Colors size fiting is very good</t>
-  </si>
-  <si>
-    <t>Fit: Regular ganesh jadhav Certified Buyer 7 months ago Lalit Kumar Certified Buyer 4 days ago</t>
-  </si>
-  <si>
-    <t>Fabric: Cotton Blend</t>
-  </si>
-  <si>
-    <t>Mid Rise Jeans</t>
-  </si>
-  <si>
-    <t>2. BEN MARTIN Slim Men Blue Je... Most Helpful Review Recent Review</t>
-  </si>
-  <si>
-    <t>3.4 115 83% Ratings &amp; 12 Reviews 1 Terrible product 1 Terrible product</t>
-  </si>
-  <si>
-    <t>₹499 off Bad product plz don't purchase Bad product plz don't purchase</t>
-  </si>
-  <si>
-    <t>Fit: Slim Flipkart Customer Certified Buyer Jan, 2022 Flipkart Customer Certified Buyer Jan, 2022</t>
-  </si>
-  <si>
-    <t>Light Fade Mid Rise Jeans</t>
-  </si>
-  <si>
-    <t>3. BEN MARTIN Regular Men Dark... Most Helpful Review Recent Review</t>
-  </si>
-  <si>
-    <t>3.7 56,64% 667 Ratings &amp; 6,727 Reviews 5 Mind-blowing purchase 3 Good</t>
-  </si>
-  <si>
-    <t>₹499 off Good product Quality , Good fitting and lovely colour. Thank you the quality is good but not as good as i expected.....</t>
-  </si>
-  <si>
-    <t>Fit: Regular flipkart team. Sachin kumar Yadav Certified Buyer 4 days ago</t>
-  </si>
-  <si>
-    <t>Fabric: Cotton Blend Debasish Gope Certified Buyer Dec, 2020</t>
-  </si>
-  <si>
-    <t>4. KOTTY Flared Women Blue Jea... Most Helpful Review Recent Review</t>
-  </si>
-  <si>
-    <t>4 4,313 75% Ratings &amp; 441 Reviews It5 's to Just gud I wowlove ! it's 4 Worth the money</t>
-  </si>
-  <si>
-    <t>₹499 off 😊 Perfect jeans but it little bit long for me</t>
-  </si>
-  <si>
-    <t>Fit: Flared Alisha11munda Munda Certified Buyer Dec, 2020 Akansha Mishra Certified Buyer 3 days ago</t>
-  </si>
-  <si>
-    <t>Fabric: Cotton Lycra Blend</t>
-  </si>
-  <si>
-    <t>High Rise Jeans</t>
-  </si>
-  <si>
-    <t>5. LEVI'S 511 Slim Men Blue Je... Most Helpful Review Recent Review</t>
-  </si>
-  <si>
-    <t>4 478 Ratings 50% &amp; 38 Reviews 5 Fabulous! 1 Worthless</t>
-  </si>
-  <si>
-    <t>₹1,599 off Levis 511 is best pair of jeans u ever get. The fitting of 511 is very I dont like this product because I want cheng but my old Flipkart</t>
-  </si>
-  <si>
-    <t>Fit: Slim classy. Love the way it's looks on my body. mobile number lost</t>
-  </si>
-  <si>
-    <t>Fabric: Cotton Blend Vishal Kumar Certified Buyer 1 month ago Radhe shyam Mochi Certified Buyer 27 days ago</t>
-  </si>
-  <si>
-    <t>Discount Men Regular Mid Rise Dark Men Skinny Mid Rise Dark</t>
-  </si>
-  <si>
-    <t>Men Slim Mid Rise Blue Men Skinny Low Rise Grey</t>
-  </si>
-  <si>
-    <t>Customer Ratings BEN Blue MARTIN BEN MARTIN Spykar Blue Roadster</t>
-  </si>
-  <si>
-    <t>Jeans Jeans Jeans Jeans</t>
-  </si>
-  <si>
-    <t>4★ &amp; above 64% 83% 60% 58% ₹499 ₹1,399 off ₹499 ₹2,999 off ₹1,479 ₹3,699 off ₹788 ₹1,899 off</t>
-  </si>
-  <si>
-    <t>3★ &amp; above Free delivery Hot Summer Deal Hot Summer Deal Free delivery</t>
-  </si>
-  <si>
-    <t>Hot Summer Deal Size  34 Size  30, 32, 34, 36, 38 Buy 2 items, save extra 5%</t>
+    <t>Mobiles &amp;</t>
+  </si>
+  <si>
+    <t>Filters Home Mobiles</t>
+  </si>
+  <si>
+    <t>Showing 1 – 24 of Accessories 167 results for "iphone14 "</t>
+  </si>
+  <si>
+    <t>Mobiles &amp; Accessories</t>
+  </si>
+  <si>
+    <t>Mobiles APPLE iPhone 24,14 (Starlight, 128 GB)</t>
+  </si>
+  <si>
+    <t>4.7 999 ₹71,692 Ratings  &amp;  976 ₹Reviews 79,900 9% off</t>
+  </si>
+  <si>
+    <t>Price 128 GB ROM Free delivery</t>
+  </si>
+  <si>
+    <t>15.49 cm (6.1 inch) Super Retina XDR Display</t>
+  </si>
+  <si>
+    <t>. . . . . 12MP + 12MP | 12MP Front Camera Upto ₹30Off Bank 000 ,on Exchange ₹30000+. A15 Bionic Chip, 6 Core Processor Processor Offer</t>
+  </si>
+  <si>
+    <t>MinMin to ₹30000+ 1 Year Warranty for Phone and 6 Months Warranty for In-Box Accessories</t>
+  </si>
+  <si>
+    <t>Brand Add to</t>
+  </si>
+  <si>
+    <t>APPLE Compare</t>
+  </si>
+  <si>
+    <t>? APPLE iPhone 24,14 (Purple, 128 GB)</t>
+  </si>
+  <si>
+    <t>Customer Ratings 128 GB ROM</t>
+  </si>
+  <si>
+    <t>4★ &amp; above 12MP + 12MP | 12MP Front Camera</t>
+  </si>
+  <si>
+    <t>3★ &amp; above A15 Bionic Chip, 6 Core Processor Processor 1 Year Warranty for Phone and 6 Months Warranty for In-Box Accessories</t>
+  </si>
+  <si>
+    <t>GST Invoice Available</t>
+  </si>
+  <si>
+    <t>Add to Compare</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>1GB and Below APPLE iPhone 14 (Blue, 128 GB)</t>
+  </si>
+  <si>
+    <t>4.7 24,692 Ratings  &amp;  976 Reviews ₹71,999 ₹79,900 9% off</t>
+  </si>
+  <si>
+    <t>Internal Storage 128 GB ROM Free delivery</t>
+  </si>
+  <si>
+    <t>15.49 cm (6.1 inch) Super Retina XDR Display Upto ₹30,000 Off on Exchange</t>
+  </si>
+  <si>
+    <t>Battery Capacity 12MP + 12MP | 12MP Front Camera Bank Offer</t>
+  </si>
+  <si>
+    <t>A15 Bionic Chip, 6 Core Processor Processor</t>
+  </si>
+  <si>
+    <t>Screen Size 1 Year Warranty for Phone and 6 Months Warranty for In-Box Accessories</t>
+  </si>
+  <si>
+    <t>Primary Camera Add to Compare</t>
+  </si>
+  <si>
+    <t>Secondary Camera</t>
+  </si>
+  <si>
+    <t>Processor Brand APPLE iPhone 14 (Midnight, 128 GB) 4.7 24,692 Ratings  &amp;  976 Reviews ₹71,999 ₹79,900 9%</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>Speciality 128 GB ROM Free delivery 15.49 cm (6.1 inch) Super Retina XDR Display Upto ₹30,000 Off on Exchange</t>
+  </si>
+  <si>
+    <t>12MP + 12MP | 12MP Front Camera Bank Offer</t>
+  </si>
+  <si>
+    <t>Resolution Type A15 Bionic Chip, 6 Core Processor Processor</t>
+  </si>
+  <si>
+    <t>1 Year Warranty for Phone and 6 Months Warranty for In-Box Accessories</t>
+  </si>
+  <si>
+    <t>Operating System</t>
+  </si>
+  <si>
+    <t>Network Type Add to Compare</t>
+  </si>
+  <si>
+    <t>Sim Type APPLE iPhone 14 ((PRODUCT)RED, 128 GB)</t>
+  </si>
+  <si>
+    <t>4.7 ₹71,999</t>
+  </si>
+  <si>
+    <t>Offers 24,692 Ratings  &amp;  976 Reviews ₹79,900 9% off</t>
+  </si>
+  <si>
+    <t>128 GB ROM Free delivery</t>
+  </si>
+  <si>
+    <t>No Cost EMI 15.49 cm (6.1 inch) Super Retina XDR Display Upto ₹30,000 Off on Exchange</t>
+  </si>
+  <si>
+    <t>Special Price 12MP + 12MP | 12MP Front Camera Bank Offer</t>
+  </si>
+  <si>
+    <t>Buy More, Save More A15 Bionic Chip, 6 Core Processor Processor 1 Year Warranty for Phone and 6 Months Warranty for In-Box Accessories</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Number of Cores APPLE iPhone 14 (Starlight, 256 GB) 4.7 24,692 Ratings  &amp;  976 Reviews ₹81,999</t>
+  </si>
+  <si>
+    <t>₹89,900 8% off</t>
+  </si>
+  <si>
+    <t>Availability 256 GB ROM Free delivery 15.49 cm (6.1 inch) Super Retina XDR Display Upto ₹30,000 Off on Exchange</t>
+  </si>
+  <si>
+    <t>Discount A15 Bionic Chip, 6 Core Processor Processor</t>
+  </si>
+  <si>
+    <t>30% or more 1 Year Warranty for Phone and 6 Months Warranty for In-Box Accessories</t>
+  </si>
+  <si>
+    <t>20% or more</t>
+  </si>
+  <si>
+    <t>10% or more Add to Compare</t>
+  </si>
+  <si>
+    <t>50% or more</t>
+  </si>
+  <si>
+    <t>40% or more APPLE iPhone 14 (Midnight, 256 GB)</t>
+  </si>
+  <si>
+    <t>4.7 24,692 Ratings  &amp;  976 Reviews ₹81,999 ₹89,900 8% off</t>
+  </si>
+  <si>
+    <t>Clock Speed 256 GB ROM Free delivery</t>
+  </si>
+  <si>
+    <t>Need help? A15 Bionic Chip, 6 Core Processor Processor</t>
+  </si>
+  <si>
+    <t>Help me decide 1 Year Warranty for Phone and 6 Months Warranty for In-Box Accessories</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 (Blue, 256 GB)</t>
+  </si>
+  <si>
+    <t>256 GB ROM Free delivery</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 ((PRODUCT)RED, 256 GB)</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 (Midnight, 512 GB)</t>
+  </si>
+  <si>
+    <t>4.7 24,692 Ratings  &amp;  976 Reviews ₹1,01,999 ₹1,09,900 7% off</t>
+  </si>
+  <si>
+    <t>512 GB ROM Free delivery</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 (Purple, 256 GB)</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 (Yellow, 128 GB)</t>
+  </si>
+  <si>
+    <t>4.7 24,692 Ratings  &amp;  976 Reviews ₹72,999 ₹79,900 8% off</t>
+  </si>
+  <si>
+    <t>15.49 cm (6.1 inch) Super Retina XDR Display Upto ₹27,000 Off on Exchange</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 (Yellow, 256 GB)</t>
+  </si>
+  <si>
+    <t>4.7 24,692 Ratings  &amp;  976 Reviews ₹82,999 ₹89,900 7% off</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 (Starlight, 512 GB)</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 (Purple, 512 GB)</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 ((PRODUCT)RED, 512 GB)</t>
+  </si>
+  <si>
+    <t>512 GB ROM</t>
+  </si>
+  <si>
+    <t>12MP + 12MP | 12MP Front Camera</t>
+  </si>
+  <si>
+    <t>Coming Soon</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 (Blue, 512 GB)</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 (Yellow, 512 GB)</t>
+  </si>
+  <si>
+    <t>4.7 24,692 Ratings  &amp;  976 Reviews ₹1,02,999 ₹1,09,900 6% off</t>
+  </si>
+  <si>
+    <t>Currently unavailable</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 Plus (Purple, 128 GB)</t>
+  </si>
+  <si>
+    <t>4.7 6,882 Ratings  &amp;  469 Reviews ₹79,999 ₹89,900 11% off</t>
+  </si>
+  <si>
+    <t>17.02 cm (6.7 inch) Super Retina XDR Display Upto ₹30,000 Off on Exchange</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 Plus (Midnight, 128 GB)</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 Plus (Starlight, 128 GB)</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 Plus ((PRODUCT)RED, 128 GB)</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 Plus (Blue, 128 GB)</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 14 Plus (Purple, 256 GB)</t>
+  </si>
+  <si>
+    <t>4.7 6,882 Ratings  &amp;  469 Reviews ₹89,999 ₹99,900 9% off</t>
+  </si>
+  <si>
+    <t>Page 1 of 7 1 2 3 4 5 6 7 Next</t>
   </si>
 </sst>
 </file>
@@ -667,560 +652,1040 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAFFCD5-9563-4C12-A74F-B88C2A336C53}">
-  <dimension ref="A1:A110"/>
+  <dimension ref="A1:A206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>